<commit_message>
updated with residential water heating load
</commit_message>
<xml_diff>
--- a/Data/load/load_data.xlsx
+++ b/Data/load/load_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\Thermal Storage\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\Thermal Storage\Data\load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F8481ED-5B3A-4A82-A0B4-471B2CB4E2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E77B29-5788-48CF-A64C-9DEB6133FF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA067B99-CC83-47CD-8733-0C1DCC6ECC84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EA067B99-CC83-47CD-8733-0C1DCC6ECC84}"/>
   </bookViews>
   <sheets>
     <sheet name="Water" sheetId="1" r:id="rId1"/>
@@ -381,84 +381,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CDFFA4-D814-49BF-8EB1-DB65A10F6A02}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2000000</v>
+        <v>0.24682862601720568</v>
       </c>
       <c r="B1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="F1">
-        <v>1000000</v>
+        <v>6.0065141685888224E-2</v>
       </c>
       <c r="G1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="H1">
-        <v>1000000</v>
+        <v>5.9144537942310671E-2</v>
       </c>
       <c r="I1">
-        <v>1000000</v>
+        <v>0.51927141127240273</v>
       </c>
       <c r="J1">
-        <v>1000000</v>
+        <v>0.52382438939645537</v>
       </c>
       <c r="K1">
-        <v>1000000</v>
+        <v>0.13038529760314024</v>
       </c>
       <c r="L1">
-        <v>1000000</v>
+        <v>0.51398284812689254</v>
       </c>
       <c r="M1">
-        <v>1000000</v>
+        <v>1.6195395117100556E-2</v>
       </c>
       <c r="N1">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="O1">
-        <v>1000000</v>
+        <v>0.26090828123027648</v>
       </c>
       <c r="P1">
-        <v>1000000</v>
+        <v>8.9361092814150195E-2</v>
       </c>
       <c r="Q1">
-        <v>1000000</v>
+        <v>1.3040826386388669E-2</v>
       </c>
       <c r="R1">
-        <v>1000000</v>
+        <v>0.2276205737539557</v>
       </c>
       <c r="S1">
-        <v>1000000</v>
+        <v>3.4640545575266177E-2</v>
       </c>
       <c r="T1">
-        <v>1000000</v>
+        <v>0.20990934955450419</v>
       </c>
       <c r="U1">
-        <v>1000000</v>
+        <v>5.4831668975116259E-2</v>
       </c>
       <c r="V1">
-        <v>1000000</v>
+        <v>0.38097232065841097</v>
       </c>
       <c r="W1">
-        <v>1000000</v>
+        <v>0.45580618727025773</v>
       </c>
       <c r="X1">
-        <v>1000000</v>
+        <v>6.1190209757303174E-2</v>
       </c>
     </row>
   </sheetData>
@@ -470,84 +470,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550FDD0A-4629-4498-B92C-E966F1141391}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>400000</v>
+        <v>0.24682862601720568</v>
       </c>
       <c r="B1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="E1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="F1">
-        <v>400000</v>
+        <v>6.0065141685888224E-2</v>
       </c>
       <c r="G1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="H1">
-        <v>400000</v>
+        <v>5.9144537942310671E-2</v>
       </c>
       <c r="I1">
-        <v>400000</v>
+        <v>0.51927141127240273</v>
       </c>
       <c r="J1">
-        <v>400000</v>
+        <v>0.52382438939645537</v>
       </c>
       <c r="K1">
-        <v>400000</v>
+        <v>0.13038529760314024</v>
       </c>
       <c r="L1">
-        <v>400000</v>
+        <v>0.51398284812689254</v>
       </c>
       <c r="M1">
-        <v>400000</v>
+        <v>1.6195395117100556E-2</v>
       </c>
       <c r="N1">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="O1">
-        <v>400000</v>
+        <v>0.26090828123027648</v>
       </c>
       <c r="P1">
-        <v>400000</v>
+        <v>8.9361092814150195E-2</v>
       </c>
       <c r="Q1">
-        <v>400000</v>
+        <v>1.3040826386388669E-2</v>
       </c>
       <c r="R1">
-        <v>400000</v>
+        <v>0.2276205737539557</v>
       </c>
       <c r="S1">
-        <v>400000</v>
+        <v>3.4640545575266177E-2</v>
       </c>
       <c r="T1">
-        <v>400000</v>
+        <v>0.20990934955450419</v>
       </c>
       <c r="U1">
-        <v>400000</v>
+        <v>5.4831668975116259E-2</v>
       </c>
       <c r="V1">
-        <v>400000</v>
+        <v>0.38097232065841097</v>
       </c>
       <c r="W1">
-        <v>400000</v>
+        <v>0.45580618727025773</v>
       </c>
       <c r="X1">
-        <v>400000</v>
+        <v>6.1190209757303174E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>